<commit_message>
Initialize and populate data steps completed
</commit_message>
<xml_diff>
--- a/YearlyReport-REFramework/Data/Config.xlsx
+++ b/YearlyReport-REFramework/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andreea.ghetu\Documents\UiPath\CSharpChanges\StudioTemplates\REFramework\C#\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andres\Repositories\RPAYearlyReport\YearlyReport-REFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96902286-4E3C-425E-A0BF-F83C72A8C5F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84191D4F-B98F-4AE8-A061-1BC9138E66A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="18000" windowHeight="9480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>ACME_Credentials</t>
+  </si>
+  <si>
+    <t>ACMELogIn</t>
   </si>
 </sst>
 </file>
@@ -541,21 +547,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18.75">
+    <row r="1" spans="1:26" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -600,7 +606,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -611,7 +617,7 @@
     <row r="4" spans="1:26">
       <c r="A4" s="7"/>
     </row>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="28.8">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -620,6 +626,14 @@
       </c>
       <c r="C5" s="4" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -633,19 +647,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18.75">
+    <row r="1" spans="1:26" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -679,23 +693,23 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>33</v>
@@ -810,7 +824,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="28.8">
       <c r="A17" s="5" t="s">
         <v>39</v>
       </c>
@@ -835,12 +849,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>